<commit_message>
final organization of lyon pilot
</commit_message>
<xml_diff>
--- a/lyon_report/supplementary_final.xlsx
+++ b/lyon_report/supplementary_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylieholt/bryo_arthro/lyon_pilot_git/lyon_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FDF0333-E5A2-F045-ABC1-819A928C40A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24698C3C-E44B-7B41-AC38-C4110C02FA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30340" yWindow="2540" windowWidth="27240" windowHeight="16440" activeTab="1" xr2:uid="{DB81101E-6613-4940-BBA1-C56FE1BF6645}"/>
+    <workbookView xWindow="-30340" yWindow="2540" windowWidth="27240" windowHeight="16440" xr2:uid="{DB81101E-6613-4940-BBA1-C56FE1BF6645}"/>
   </bookViews>
   <sheets>
     <sheet name="supplementary_final" sheetId="1" r:id="rId1"/>
@@ -5005,7 +5005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E5AE6A8-3450-6947-AB69-3552F5CA11D3}">
   <dimension ref="A1:P781"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -44070,7 +44070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD53F83D-849D-AE4B-BC89-EDF6360004B7}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>